<commit_message>
cached embedding model, E135 added
</commit_message>
<xml_diff>
--- a/preprocessing/data/all-in-transcripts/cleaned/E134_sections_full_cleaned.xlsx
+++ b/preprocessing/data/all-in-transcripts/cleaned/E134_sections_full_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielfurman/Desktop/github_repos/chat-all-in-hf/preprocessing/data/all-in-transcripts/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE5D6D5-CB77-D747-800B-EB0185F21E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B3AD2-8B1C-7B41-8676-C505F1F3174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="1140" windowWidth="24720" windowHeight="17280" xr2:uid="{DB6335B9-F6CB-404A-8475-8E90C4B96651}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Bestie intros!: Bad conference lunches, hair fluffers, and focus groups</t>
   </si>
@@ -96,9 +96,6 @@
     <t>E134: Ukraine counteroffensive, China tensions, COVID Patient Zero, RFK Jr reaction &amp; more</t>
   </si>
   <si>
-    <t>section_summary</t>
-  </si>
-  <si>
     <t>episode_title</t>
   </si>
   <si>
@@ -109,27 +106,6 @@
   </si>
   <si>
     <t>section_time_stamp</t>
-  </si>
-  <si>
-    <t>In this section, the hosts discuss their experiences at various conferences and summits, including the Kotu conference and Coaching Summit. They comment on the sober and somber vibe of the events, reflecting on the challenges faced by tech companies and the impact of the Federal Reserve's actions on business behavior. They also mention the importance of maintaining the podcast's formula and chemistry, as confirmed by feedback from a Netflix employee who appreciates the back-and-forth dynamic of the hosts. Additionally, they make lighthearted remarks about conference lunches, haircuts, and fashion choices.</t>
-  </si>
-  <si>
-    <t>In this section, the hosts engage in a playful conversation about the physical fitness of Mark Zuckerberg and Elon Musk. They discuss Zuck's dedication to training in mixed martial arts and Musk's past neck injury from a sumo wrestling match. The hosts humorously debate the idea of a cage match between the two tech moguls, with contrasting opinions on who would come out on top. The conversation veers into discussing the financial performance of their respective companies, Twitter and Tesla, with playful analogies and banter.</t>
-  </si>
-  <si>
-    <t>In this section, the hosts discuss the ongoing conflict between Russia and Ukraine. They analyze the underwhelming progress of Ukraine's counter-offensive and the potential rejection of a peace deal by the West. The conversation delves into the military dynamics, including the fortified lines and obstacles set up by Russia, as well as the depletion of ammunition and the implications of the conflict on the global stage. They emphasize the need for open discussions and critical thinking regarding Ukraine and other geopolitical issues.</t>
-  </si>
-  <si>
-    <t>In this section, the hosts discussed Secretary of State Antony Blinken's recent visit to China, highlighting the strained relationship between the two countries. They criticized President Biden's remark referring to Xi Jinping as a dictator during a fundraiser in California, questioning the impact of undisciplined statements on diplomatic efforts. The conversation also touched on the need for collaboration and engagement with China on global issues, such as climate change, while expressing concerns about the potential vulnerability of Taiwan and the importance of maintaining the status quo.</t>
-  </si>
-  <si>
-    <t>The transcript is a section from the "All-In" podcast discussing the heating up of the secondary market for depressed startup shares. They explain that secondary markets involve one investor buying shares in a private company directly from another investor on the cap table. They discuss how some firms, including Tiger Global, are offering shares in their portfolio companies at discounted prices, with shares of startups trading at a median discount of 61% compared to their latest funding rounds. The hosts analyze the repricing of unprofitable tech companies in both public and private markets and anticipate an increase in market clearing events as companies need to raise capital and employees seek liquidity.</t>
-  </si>
-  <si>
-    <t>The transcript is a section from the "All-In" podcast discussing Ford's $9.2 billion federal loan from the U.S. Department of Energy to build three EV battery factories. The loan is aimed at onshoring and reshoring manufacturing and reducing the country's dependence on fossil fuels. The hosts debate the merits of industrial policy and government intervention, with some supporting it as a way to achieve energy independence and national security, while others raise concerns about crony capitalism and the potential inefficiency of government investments. They also discuss the market demand for Ford's EVs and the need for risk capital and participation in the upside for government loans.</t>
-  </si>
-  <si>
-    <t>The transcript is a section from the "All-In" podcast discussing various topics, including RFK Jr.'s appearance on Joe Rogan's podcast, the influence of big pharma on media through advertising, and the origins of COVID-19. The hosts clarify that while some members of the podcast may have hosted a fundraiser for RFK Jr., it doesn't imply unanimous support. They express support for RFK Jr. on issues such as free speech, civil liberties, and peace but also acknowledge disagreement on topics like nuclear energy and anti-vaccine stance. They criticize media's control over public opinion and the lack of thorough investigative reporting, particularly when it comes to questioning pharma companies and COVID-19 origins.</t>
   </si>
   <si>
     <t>Jun 23, 2023</t>
@@ -502,29 +478,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{602A8643-EBB0-AE42-81C3-FC24B888747B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="93" customWidth="1"/>
     <col min="2" max="2" width="35.1640625" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
@@ -532,11 +508,8 @@
       <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -547,16 +520,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -567,16 +537,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -586,17 +553,14 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -607,16 +571,13 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -626,17 +587,14 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -646,17 +604,14 @@
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -666,14 +621,11 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
+      <c r="E8" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>